<commit_message>
update trees/stacks notes, update excel comparison chart
</commit_message>
<xml_diff>
--- a/Data_Structures.xlsx
+++ b/Data_Structures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbildner/Library/Containers/com.microsoft.Excel/Data/Desktop/AA-Data-Structures-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB167CA-29DF-954E-895F-1D57B2411F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22F6F0-167C-4745-9AF6-B410E0BAEA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="460" windowWidth="33360" windowHeight="23540" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
+    <workbookView xWindow="3780" yWindow="460" windowWidth="31040" windowHeight="26300" activeTab="2" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Light Blank" sheetId="8" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Table" sheetId="2" r:id="rId3"/>
     <sheet name="DSA Pros Cons Light" sheetId="5" r:id="rId4"/>
     <sheet name="DSA Pros Cons Dark" sheetId="4" r:id="rId5"/>
+    <sheet name="DS Applications" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
   <si>
     <t>Arrays</t>
   </si>
@@ -1304,15 +1305,67 @@
   </si>
   <si>
     <t xml:space="preserve">  not preserved unlike arrays</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>STACKS</t>
+  </si>
+  <si>
+    <t>BackTracking</t>
+  </si>
+  <si>
+    <t>Browsing History (React Router Module)</t>
+  </si>
+  <si>
+    <t>Undo/Redo Functionality</t>
+  </si>
+  <si>
+    <t>Syntax/Parenthesis Parsing</t>
+  </si>
+  <si>
+    <t>Reversing Things (ex. A string)</t>
+  </si>
+  <si>
+    <t>Function Calls</t>
+  </si>
+  <si>
+    <t>Operating systems to keep track of active functions/subroutines</t>
+  </si>
+  <si>
+    <t>QUEUES</t>
+  </si>
+  <si>
+    <t>Breadth First Search (BFS) Traversing</t>
+  </si>
+  <si>
+    <t>Operating systems to handle job scheduling</t>
+  </si>
+  <si>
+    <t>Chat rooms, customer service phone lines</t>
+  </si>
+  <si>
+    <t>Amazon's Simple Queue Service (Part of AWS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1927,91 +1980,94 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dark Mode" xfId="1" xr:uid="{C2D7DBCB-6819-4E7C-B7AB-3B87B9FAFFF0}"/>
@@ -2330,10 +2386,10 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -2467,13 +2523,39 @@
       <c r="I11" s="74"/>
       <c r="J11" s="74"/>
     </row>
-    <row r="17" spans="1:1" ht="16">
-      <c r="A17" s="56" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="74"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="74"/>
+    </row>
+    <row r="21" spans="1:1" ht="16">
+      <c r="A21" s="56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16">
-      <c r="A18" s="56" t="s">
+    <row r="22" spans="1:1" ht="16">
+      <c r="A22" s="56" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2488,10 +2570,10 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -2603,7 +2685,7 @@
       </c>
       <c r="F7" s="70"/>
       <c r="G7" s="68" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H7" s="69" t="s">
         <v>8</v>
@@ -2751,13 +2833,71 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16">
-      <c r="A22" s="56" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16">
+      <c r="A30" s="56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16">
-      <c r="A23" s="56" t="s">
+    <row r="31" spans="1:10" ht="16">
+      <c r="A31" s="56" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2770,10 +2910,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497D1617-BE90-5941-97A0-B0844D3A8488}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -2883,7 +3023,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>8</v>
@@ -2980,7 +3120,7 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3008,73 +3148,133 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16">
-      <c r="A30" s="18" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16">
+      <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3">
-        <v>4000</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>29</v>
+    <row r="31" spans="1:10" ht="16">
+      <c r="A31" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3">
-        <v>1200</v>
+        <v>5000</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="3">
-        <v>1100</v>
-      </c>
       <c r="B35" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3">
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3">
-        <v>1160</v>
+        <v>1100</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3">
+        <v>1160</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3">
-        <f>SUM(A32:A38)</f>
-        <v>9760</v>
+        <v>200</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="3">
+        <f>SUM(A34:A40)</f>
+        <v>8760</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3350,7 +3550,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -3681,4 +3881,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E0F671-BDD6-AC46-B055-4342B924FD5C}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A49" r:id="rId1" display="https://www.faceprep.in/procoder/knowledgebase/advantages-and-disadvantages-of-arrays/" xr:uid="{ABF5AD01-8BAB-0649-BCCB-786CB64032A8}"/>
+    <hyperlink ref="A50" r:id="rId2" display="https://www.metaltoad.com/blog/javascript-understanding-objects-vs-arrays-and-when-use-them-part-1" xr:uid="{AB46E4CC-741B-3041-92D2-83658DECBB7F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
practice tree traversal iterative/recursive algos, update BST/Tree notes
</commit_message>
<xml_diff>
--- a/Data_Structures.xlsx
+++ b/Data_Structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbildner/Library/Containers/com.microsoft.Excel/Data/Desktop/AA-Data-Structures-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22F6F0-167C-4745-9AF6-B410E0BAEA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EEA9A3-1E47-084B-BE7A-9C3D5FCDE42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="31040" windowHeight="26300" activeTab="2" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
+    <workbookView xWindow="2620" yWindow="460" windowWidth="27580" windowHeight="24560" activeTab="6" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Light Blank" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="DSA Pros Cons Light" sheetId="5" r:id="rId4"/>
     <sheet name="DSA Pros Cons Dark" sheetId="4" r:id="rId5"/>
     <sheet name="DS Applications" sheetId="10" r:id="rId6"/>
+    <sheet name="Binary Trees vs BST" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="109">
   <si>
     <t>Arrays</t>
   </si>
@@ -1351,12 +1352,48 @@
   <si>
     <t>Amazon's Simple Queue Service (Part of AWS)</t>
   </si>
+  <si>
+    <t>BINARY SEARCH TREES</t>
+  </si>
+  <si>
+    <t>TREES</t>
+  </si>
+  <si>
+    <t>AVL TREES</t>
+  </si>
+  <si>
+    <t>HEAPS</t>
+  </si>
+  <si>
+    <t>TRIES</t>
+  </si>
+  <si>
+    <t>BINARY TREE</t>
+  </si>
+  <si>
+    <t>BINARY SEARCH TREE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - each node has at most 2 children</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - has 1 root node</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - directed edges (one way)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - for any node, values in left subtree must all be &lt; nodes value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - for any node, values in right subtree must all be &gt;= nodes value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1566,6 +1603,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1982,7 +2026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2068,6 +2112,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dark Mode" xfId="1" xr:uid="{C2D7DBCB-6819-4E7C-B7AB-3B87B9FAFFF0}"/>
@@ -2912,7 +2957,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -3888,7 +3933,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -3979,60 +4024,75 @@
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D16" s="21"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D17" s="21"/>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D18" s="21"/>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="1:4">
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="1:4">
       <c r="D20" s="21"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="1:4">
       <c r="D21" s="21"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="1:4">
       <c r="D22" s="21"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="1:4">
       <c r="D23" s="21"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="1:4">
       <c r="D24" s="21"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="1:4">
       <c r="D25" s="21"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="1:4">
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="1:4">
       <c r="D27" s="21"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="1:4">
       <c r="D28" s="21"/>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="1:4">
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="4:4">
+    <row r="30" spans="1:4">
       <c r="D30" s="21"/>
     </row>
-    <row r="31" spans="4:4">
+    <row r="31" spans="1:4">
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="4:4">
+    <row r="32" spans="1:4">
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="4:4">
@@ -4049,4 +4109,163 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87EF43E-316E-8E49-808C-D3A9E3E622B1}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A49" r:id="rId1" display="https://www.faceprep.in/procoder/knowledgebase/advantages-and-disadvantages-of-arrays/" xr:uid="{D56EE712-CD29-724E-9C1C-DA909723A0E3}"/>
+    <hyperlink ref="A50" r:id="rId2" display="https://www.metaltoad.com/blog/javascript-understanding-objects-vs-arrays-and-when-use-them-part-1" xr:uid="{E747BFDB-A92A-4049-8FED-827B53D19C01}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update bst pros/cons/when to use
</commit_message>
<xml_diff>
--- a/Data_Structures.xlsx
+++ b/Data_Structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbildner/Library/Containers/com.microsoft.Excel/Data/Desktop/AA-Data-Structures-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EEA9A3-1E47-084B-BE7A-9C3D5FCDE42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFB79C7-8DB8-1445-903C-5FDA566723A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="27580" windowHeight="24560" activeTab="6" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
+    <workbookView xWindow="11180" yWindow="460" windowWidth="34800" windowHeight="27580" activeTab="3" xr2:uid="{0393503C-83F5-471D-900E-F1C45181E793}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Light Blank" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="125">
   <si>
     <t>Arrays</t>
   </si>
@@ -1388,12 +1388,130 @@
   <si>
     <t xml:space="preserve"> - for any node, values in right subtree must all be &gt;= nodes value</t>
   </si>
+  <si>
+    <t>Binary Search Tree</t>
+  </si>
+  <si>
+    <t>O(log(N))</t>
+  </si>
+  <si>
+    <t>^best/average case happens if tree is balanced</t>
+  </si>
+  <si>
+    <t>^worst case if tree is NOT balanced</t>
+  </si>
+  <si>
+    <t>Dictionary (fast lookup for words)</t>
+  </si>
+  <si>
+    <t>Huffman Compression Algorithm</t>
+  </si>
+  <si>
+    <t>Search Algorithm</t>
+  </si>
+  <si>
+    <t>Multilevel indexing in data bases</t>
+  </si>
+  <si>
+    <t>Stacks &amp; Queues</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Simple, and very fast insert/deletion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Time for back(stack)/front(queue) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Access and Search are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O(N)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Fast Access/Search Average Time Complexity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O(log(N))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if tree is balanced</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Search Trees </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Ultimate "average" data structure/well balanced because all average time operations are O(log(N))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - range searches (ex. find all elements between 0-32) more efficient than HashTable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - All operations are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O(N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Worst Case Time Complexity if tree is NOT balanced</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1611,6 +1729,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1638,7 +1781,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -2021,12 +2164,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2113,6 +2283,25 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dark Mode" xfId="1" xr:uid="{C2D7DBCB-6819-4E7C-B7AB-3B87B9FAFFF0}"/>
@@ -2434,12 +2623,12 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="54" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="54" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="54" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="54" customWidth="1"/>
@@ -2594,12 +2783,25 @@
       <c r="I15" s="77"/>
       <c r="J15" s="74"/>
     </row>
-    <row r="21" spans="1:1" ht="16">
+    <row r="17" spans="1:10">
+      <c r="A17" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="74"/>
+    </row>
+    <row r="21" spans="1:10" ht="16">
       <c r="A21" s="56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16">
+    <row r="22" spans="1:10" ht="16">
       <c r="A22" s="56" t="s">
         <v>76</v>
       </c>
@@ -2618,12 +2820,12 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="54" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="54" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="54" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" style="54" customWidth="1"/>
@@ -2934,6 +3136,43 @@
       </c>
       <c r="J23" s="68" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16">
@@ -2958,12 +3197,12 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="3" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" style="3" customWidth="1"/>
@@ -3251,6 +3490,43 @@
         <v>7</v>
       </c>
     </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="30" spans="1:10" ht="16">
       <c r="A30" s="3" t="s">
         <v>22</v>
@@ -3334,10 +3610,10 @@
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -3569,21 +3845,135 @@
       </c>
       <c r="C32" s="43"/>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="42" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="85"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="91"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="93"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="89" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="89"/>
+      <c r="B36" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="90"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="89"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="94" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="89"/>
+      <c r="B41" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="34">
+      <c r="A42" s="89"/>
+      <c r="B42" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="87"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="89"/>
+      <c r="B43" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="87"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="90"/>
+      <c r="B44" s="86"/>
+      <c r="C44" s="86"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="89"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="94" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="89"/>
+      <c r="B48" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="34">
+      <c r="A49" s="89"/>
+      <c r="B49" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="87"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="89"/>
+      <c r="B50" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="87"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="42" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" s="42" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A49" r:id="rId1" display="https://www.faceprep.in/procoder/knowledgebase/advantages-and-disadvantages-of-arrays/" xr:uid="{D64382EE-6FA4-F047-A7B6-00DF7B6A7213}"/>
-    <hyperlink ref="A50" r:id="rId2" display="https://www.metaltoad.com/blog/javascript-understanding-objects-vs-arrays-and-when-use-them-part-1" xr:uid="{6D990E39-34E1-A94C-AC0C-475FCC080153}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3592,10 +3982,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3B6200-D14D-B646-BEE4-89986D7A14A7}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -3897,24 +4287,136 @@
       <c r="C32" s="24"/>
       <c r="D32" s="21"/>
     </row>
-    <row r="33" spans="1:4">
-      <c r="D33" s="21"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="20" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="82"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="27"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="25"/>
+      <c r="B36" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="82"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="83" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="25"/>
+      <c r="B40" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="34">
+      <c r="A41" s="25"/>
+      <c r="B41" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="25"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="82"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="83" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="25"/>
+      <c r="B46" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="34">
+      <c r="A47" s="25"/>
+      <c r="B47" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="25"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="25"/>
+      <c r="B48" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="25"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="80"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="20" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="20" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3933,7 +4435,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -4033,23 +4535,26 @@
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>100</v>
+      <c r="B16" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>99</v>
+      <c r="B17" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>101</v>
+      <c r="B18" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="D18" s="21"/>
     </row>
@@ -4066,12 +4571,21 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4">
@@ -4115,8 +4629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87EF43E-316E-8E49-808C-D3A9E3E622B1}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>

</xml_diff>